<commit_message>
averages added to temp calibration data
</commit_message>
<xml_diff>
--- a/Calibration/tempCalibrationData.xlsx
+++ b/Calibration/tempCalibrationData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\whits\STUFF\SCHOOL\ME121-Fishtank\Calibration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB23114-4124-4003-9906-C24B7958038E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CAB90C4-92EF-4323-A4B1-6A90024FABCA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{54487774-316F-4B11-9400-23F4EBD6C940}"/>
   </bookViews>
@@ -33,16 +33,19 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t xml:space="preserve"> Temp C</t>
+  </si>
+  <si>
+    <t>Avrg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -52,6 +55,14 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -79,9 +90,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -396,16 +408,63 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91C169E9-91DA-46AB-B124-2303AFC055B5}">
-  <dimension ref="A2:L69"/>
+  <dimension ref="A1:L69"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1">
+        <f>AVERAGE(B3:B69)</f>
+        <v>842.82089552238801</v>
+      </c>
+      <c r="C1">
+        <f>AVERAGE(C3:C69)</f>
+        <v>849.8955223880597</v>
+      </c>
+      <c r="D1">
+        <f>AVERAGE(D3:D69)</f>
+        <v>777.1044776119403</v>
+      </c>
+      <c r="E1">
+        <f>AVERAGE(E3:E69)</f>
+        <v>503.05970149253733</v>
+      </c>
+      <c r="F1">
+        <f>AVERAGE(F3:F69)</f>
+        <v>493.71641791044777</v>
+      </c>
+      <c r="G1">
+        <f>AVERAGE(G3:G69)</f>
+        <v>576.32835820895525</v>
+      </c>
+      <c r="H1">
+        <f>AVERAGE(H3:H69)</f>
+        <v>646.08955223880594</v>
+      </c>
+      <c r="I1">
+        <f>AVERAGE(I3:I69)</f>
+        <v>726.74626865671644</v>
+      </c>
+      <c r="J1">
+        <f>AVERAGE(J3:J69)</f>
+        <v>891.67164179104475</v>
+      </c>
+      <c r="K1">
+        <f>AVERAGE(K3:K69)</f>
+        <v>742.91044776119406</v>
+      </c>
+      <c r="L1">
+        <f>AVERAGE(L3:L69)</f>
+        <v>677.97014925373139</v>
+      </c>
+    </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="1">

</xml_diff>